<commit_message>
Add missing example file
</commit_message>
<xml_diff>
--- a/static/files/listing_bailleur.xlsx
+++ b/static/files/listing_bailleur.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pitou/Pro/apilos/apilos_settings/tests/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pitou/Pro/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1822726-DF8D-F24B-A307-711300DE54FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2B7384-0FDE-BF44-9D8A-D82C52F43260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="500" windowWidth="34980" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,9 +32,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -1364,13 +1367,13 @@
     <t>bruno.duquenoy@nord.gouv.fr</t>
   </si>
   <si>
-    <t>Bailleur HLM de test</t>
-  </si>
-  <si>
-    <t>L'Autre</t>
-  </si>
-  <si>
-    <t>sabine@apilos.com</t>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Nom complet Bailleur</t>
+  </si>
+  <si>
+    <t>jean.martin@bailleur.gouv</t>
   </si>
 </sst>
 </file>
@@ -2246,8 +2249,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3449,6 +3452,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-EF11-644C-AD45-9B0FACA587B7}"/>
                 </c:ext>
@@ -3480,6 +3484,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-EF11-644C-AD45-9B0FACA587B7}"/>
                 </c:ext>
@@ -3511,6 +3516,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-EF11-644C-AD45-9B0FACA587B7}"/>
                 </c:ext>
@@ -3797,6 +3803,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-B7AD-514F-AD48-CE45DC496372}"/>
                 </c:ext>
@@ -3828,6 +3835,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-B7AD-514F-AD48-CE45DC496372}"/>
                 </c:ext>
@@ -3859,6 +3867,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-B7AD-514F-AD48-CE45DC496372}"/>
                 </c:ext>
@@ -4179,6 +4188,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-45F6-C541-8F65-A82ED2200461}"/>
                 </c:ext>
@@ -4210,6 +4220,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-45F6-C541-8F65-A82ED2200461}"/>
                 </c:ext>
@@ -4241,6 +4252,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-45F6-C541-8F65-A82ED2200461}"/>
                 </c:ext>
@@ -4272,6 +4284,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-45F6-C541-8F65-A82ED2200461}"/>
                 </c:ext>
@@ -4303,6 +4316,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-45F6-C541-8F65-A82ED2200461}"/>
                 </c:ext>
@@ -4618,6 +4632,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-6200-FC47-BC40-A89F137DFDBA}"/>
                 </c:ext>
@@ -4649,6 +4664,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-6200-FC47-BC40-A89F137DFDBA}"/>
                 </c:ext>
@@ -4680,6 +4696,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-6200-FC47-BC40-A89F137DFDBA}"/>
                 </c:ext>
@@ -4711,6 +4728,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-6200-FC47-BC40-A89F137DFDBA}"/>
                 </c:ext>
@@ -5434,7 +5452,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15"/>
@@ -5478,13 +5496,13 @@
     </row>
     <row r="2" spans="1:8" ht="42" customHeight="1">
       <c r="A2" s="95" t="s">
-        <v>153</v>
+        <v>433</v>
       </c>
       <c r="B2" s="95" t="s">
+        <v>433</v>
+      </c>
+      <c r="C2" s="98" t="s">
         <v>434</v>
-      </c>
-      <c r="C2" s="98" t="s">
-        <v>433</v>
       </c>
       <c r="D2" s="97"/>
       <c r="E2" s="95"/>

</xml_diff>